<commit_message>
updated agenda spreadsheet and checklist
</commit_message>
<xml_diff>
--- a/FY22/CE-QUAL-W2/CE-QUAL-W2_Workshop_Agenda_Aug_2022_Checklist.xlsx
+++ b/FY22/CE-QUAL-W2/CE-QUAL-W2_Workshop_Agenda_Aug_2022_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/GitHub/environmentalsystems/Workshops/FY22/CE-QUAL-W2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F93D0-2699-0B40-B999-8EC8C558C149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88144050-5564-614D-85C1-9FB2115E22E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7D882646-A55C-4A5C-840E-5C8671CF37BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
   <si>
     <t>Lecture 1.6</t>
   </si>
@@ -147,21 +147,12 @@
     <t>New Features in V4.5</t>
   </si>
   <si>
-    <t>CE-QUAL-W2 Control File</t>
-  </si>
-  <si>
-    <t>Model Setup and Input Data</t>
-  </si>
-  <si>
     <t>Water Temperature</t>
   </si>
   <si>
     <t>Model Utilities</t>
   </si>
   <si>
-    <t xml:space="preserve"> Model Utilities</t>
-  </si>
-  <si>
     <t>Calibration &amp; Validation Fundamentals</t>
   </si>
   <si>
@@ -208,6 +199,63 @@
   </si>
   <si>
     <t>Co-Instructor</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Output Review</t>
+  </si>
+  <si>
+    <t>Model Setup (Control File)</t>
+  </si>
+  <si>
+    <t>To do: Create slides from Word doc</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>&lt;--- 1 student has questions; Bernadel?</t>
+  </si>
+  <si>
+    <t>Todd's Tasks</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Send final agenda</t>
+  </si>
+  <si>
+    <t>Ask for suggestions for special topics</t>
+  </si>
+  <si>
+    <t>Send instructions for installing software</t>
+  </si>
+  <si>
+    <t>Send links</t>
   </si>
 </sst>
 </file>
@@ -312,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,26 +383,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,9 +733,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574DED2A-EF5B-6E4C-8950-1752772D8394}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -686,11 +745,13 @@
     <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.83203125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="8" width="11.1640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="9.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.83203125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -704,19 +765,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -730,11 +803,18 @@
         <v>17</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -748,11 +828,18 @@
         <v>17</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -763,16 +850,23 @@
         <v>34</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -786,11 +880,18 @@
         <v>18</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -804,34 +905,48 @@
         <v>19</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>16</v>
@@ -840,49 +955,70 @@
         <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="I8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="B9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -896,11 +1032,18 @@
         <v>18</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -914,11 +1057,21 @@
         <v>19</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -934,11 +1087,18 @@
       <c r="E13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -952,13 +1112,20 @@
         <v>18</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -966,19 +1133,26 @@
         <v>27</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -986,19 +1160,26 @@
         <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -1006,7 +1187,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>18</v>
@@ -1014,147 +1195,235 @@
       <c r="E17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="I17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>2</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>3</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
-        <v>3</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>3</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="I21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
         <v>3</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="B22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="28" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="16">
+        <v>44781</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="17">
+        <v>44781</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A24:K24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>